<commit_message>
commit after starting abalone
</commit_message>
<xml_diff>
--- a/graphs.xlsx
+++ b/graphs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="94">
   <si>
     <t>State-gov</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Never-worked</t>
+  </si>
+  <si>
+    <t>Missing</t>
   </si>
   <si>
     <t>Missing values</t>
@@ -371,39 +374,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.27009601924759408"/>
+          <c:y val="0.14351851851851852"/>
+          <c:w val="0.68668175853018376"/>
+          <c:h val="0.63759988334791484"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
@@ -629,6 +612,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>workclass</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -694,6 +732,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>% of total</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -739,6 +832,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.44310586176727912"/>
+          <c:y val="5.150408282298042E-2"/>
+          <c:w val="0.2026771653543307"/>
+          <c:h val="7.8125546806649182E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -819,39 +922,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12548381452318461"/>
+          <c:y val="0.18055555555555552"/>
+          <c:w val="0.84396062992125986"/>
+          <c:h val="0.63759988334791484"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -1164,6 +1247,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>education-num</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1229,6 +1367,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>% of total</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1274,6 +1467,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.40977252843394574"/>
+          <c:y val="7.4652230971128566E-2"/>
+          <c:w val="0.2026771653543307"/>
+          <c:h val="7.8125546806649182E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1354,39 +1557,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.33787335958005249"/>
+          <c:y val="0.19907407407407407"/>
+          <c:w val="0.61890441819772524"/>
+          <c:h val="0.63759988334791484"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
@@ -1588,6 +1771,68 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>marital-status</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1653,6 +1898,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>% of total</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1698,6 +1998,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.39032808398950131"/>
+          <c:y val="8.8541119860017448E-2"/>
+          <c:w val="0.2026771653543307"/>
+          <c:h val="7.8125546806649182E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1778,39 +2088,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.29366535433070867"/>
+          <c:y val="0.13102444012680234"/>
+          <c:w val="0.66589020122484688"/>
+          <c:h val="0.72388562540793511"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
@@ -2108,6 +2398,68 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>occupation</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2173,6 +2525,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>% of total</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2218,6 +2625,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.40699475065616797"/>
+          <c:y val="5.1586884972711806E-2"/>
+          <c:w val="0.2026771653543307"/>
+          <c:h val="5.8441967481337571E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2298,37 +2715,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2521,6 +2908,76 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>relationship</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.49695013123359583"/>
+              <c:y val="0.77277704870224551"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2586,6 +3043,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>%</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> of total</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2711,39 +3228,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.24783158355205595"/>
+          <c:y val="0.11574074074074074"/>
+          <c:w val="0.7026128608923885"/>
+          <c:h val="0.6857999104302922"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
@@ -2921,6 +3418,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>race</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2986,6 +3538,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>%</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> of total</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3031,6 +3643,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.39866141732283467"/>
+          <c:y val="5.6133712452610049E-2"/>
+          <c:w val="0.2026771653543307"/>
+          <c:h val="7.6661510923641124E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3111,39 +3733,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12548381452318461"/>
+          <c:y val="0.20370370370370369"/>
+          <c:w val="0.84396062992125986"/>
+          <c:h val="0.63759988334791484"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -3286,6 +3888,68 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>sex</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3351,6 +4015,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>% of total</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3396,6 +4115,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.3958836395450569"/>
+          <c:y val="7.4652230971128566E-2"/>
+          <c:w val="0.2026771653543307"/>
+          <c:h val="7.8125546806649182E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3476,39 +4205,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.39183267716535436"/>
+          <c:y val="7.0417750513148705E-2"/>
+          <c:w val="0.57127843394575673"/>
+          <c:h val="0.86741269709328883"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
@@ -4118,6 +4827,68 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>native-country</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4183,6 +4954,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>%</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> of total</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4215,6 +5046,836 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="650303632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.38477252843394577"/>
+          <c:y val="2.626641133653192E-2"/>
+          <c:w val="0.2026771653543307"/>
+          <c:h val="2.8142780548318973E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$176</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>&lt;=50K</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$177:$C$216</c:f>
+              <c:strCache>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>Guatemala</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Scotland</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Laos</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Trinadad&amp;Tobago</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Missing</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Cambodia</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Canada</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>China</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Columbia</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Cuba</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Dominican-Republic</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Ecuador</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>El-Salvador</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>England</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>France</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Germany</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Greece</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Haiti</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Honduras</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Hong</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Hungary</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>India</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Iran</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Ireland</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Italy</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Jamaica</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Japan</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Mexico</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Nicaragua</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Outlying-US(Guam-USVI-etc)</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Peru</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Philippines</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Poland</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Portugal</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Puerto-Rico</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>South</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Taiwan</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Thailand</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Vietnam</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>Yugoslavia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$177:$D$216</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>9.7000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6400000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0199999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.2300000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.80900000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.8299999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.14960000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.12540000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.7000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.13750000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.12130000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.0600000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.19009999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.09E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.0199999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.22239999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.0399999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.1051</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.4199999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.2300000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.21E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.1173</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.8500000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.8299999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.2999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8.09E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.8900000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.1893</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.6599999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.2300000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.2499999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.29530000000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8.8900000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8.8900000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.25080000000000002</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.12540000000000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.2300000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.0399999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6.8699999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.0199999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0E53-4428-8C3B-BFE44BC50A46}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$176</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>&gt;50K</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$177:$C$216</c:f>
+              <c:strCache>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>Guatemala</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Scotland</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Laos</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Trinadad&amp;Tobago</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Missing</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Cambodia</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Canada</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>China</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Columbia</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Cuba</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Dominican-Republic</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Ecuador</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>El-Salvador</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>England</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>France</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Germany</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Greece</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Haiti</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Honduras</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Hong</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Hungary</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>India</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Iran</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Ireland</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Italy</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Jamaica</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Japan</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Mexico</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Nicaragua</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Outlying-US(Guam-USVI-etc)</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Peru</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Philippines</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Poland</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Portugal</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Puerto-Rico</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>South</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Taiwan</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Thailand</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Vietnam</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>Yugoslavia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$177:$E$216</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.94369999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5499999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.30599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.20399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.5499999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1147</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.8199999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.5499999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.5499999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.21679999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.0999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.17849999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.1275</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.3700000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.2699999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.5499999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.8199999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.28050000000000003</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.0999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7.6499999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.1147</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.3700000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.10199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.17849999999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.2699999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.2699999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.5499999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.30599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6.3700000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.10199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.10199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5.0999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7.6499999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.5499999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.5499999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.5499999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0E53-4428-8C3B-BFE44BC50A46}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="720519184"/>
+        <c:axId val="720513936"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="720519184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="720513936"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="720513936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="720519184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4614,6 +6275,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -8144,6 +9845,511 @@
 </file>
 
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8763,13 +10969,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>76</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8841,7 +11047,7 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
       <xdr:row>110</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8933,6 +11139,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>514349</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EB5D968-D01B-4CCD-83EB-010AA5EDFC56}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9238,10 +11480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:E172"/>
+  <dimension ref="C4:E216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C131" sqref="C131:E172"/>
+    <sheetView tabSelected="1" topLeftCell="F130" workbookViewId="0">
+      <selection activeCell="V172" sqref="V172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9295,7 +11537,7 @@
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8">
         <v>6.6544999999999996</v>
@@ -9361,7 +11603,7 @@
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D21" t="s">
         <v>8</v>
@@ -9548,7 +11790,7 @@
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D41" t="s">
         <v>8</v>
@@ -9559,7 +11801,7 @@
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D42">
         <v>16.100300000000001</v>
@@ -9570,7 +11812,7 @@
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D43">
         <v>5.2499999999999998E-2</v>
@@ -9581,7 +11823,7 @@
     </row>
     <row r="44" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D44">
         <v>33.511299999999999</v>
@@ -9592,7 +11834,7 @@
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D45">
         <v>1.5532999999999999</v>
@@ -9603,7 +11845,7 @@
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D46">
         <v>41.229700000000001</v>
@@ -9614,7 +11856,7 @@
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D47">
         <v>3.8794</v>
@@ -9625,7 +11867,7 @@
     </row>
     <row r="48" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D48">
         <v>3.6730999999999998</v>
@@ -9636,7 +11878,7 @@
     </row>
     <row r="59" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D59" t="s">
         <v>8</v>
@@ -9647,7 +11889,7 @@
     </row>
     <row r="60" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D60">
         <v>6.6828000000000003</v>
@@ -9658,7 +11900,7 @@
     </row>
     <row r="61" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D61">
         <v>13.1998</v>
@@ -9669,7 +11911,7 @@
     </row>
     <row r="62" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D62">
         <v>3.2300000000000002E-2</v>
@@ -9680,7 +11922,7 @@
     </row>
     <row r="63" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D63">
         <v>12.823600000000001</v>
@@ -9691,7 +11933,7 @@
     </row>
     <row r="64" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D64">
         <v>8.4870000000000001</v>
@@ -9702,7 +11944,7 @@
     </row>
     <row r="65" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D65">
         <v>3.5558000000000001</v>
@@ -9713,7 +11955,7 @@
     </row>
     <row r="66" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D66">
         <v>5.1940999999999997</v>
@@ -9724,7 +11966,7 @@
     </row>
     <row r="67" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D67">
         <v>7.0872999999999999</v>
@@ -9735,7 +11977,7 @@
     </row>
     <row r="68" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D68">
         <v>12.775</v>
@@ -9746,7 +11988,7 @@
     </row>
     <row r="69" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D69">
         <v>0.59870000000000001</v>
@@ -9757,7 +11999,7 @@
     </row>
     <row r="70" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D70">
         <v>9.2272999999999996</v>
@@ -9768,7 +12010,7 @@
     </row>
     <row r="71" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D71">
         <v>1.7718</v>
@@ -9779,7 +12021,7 @@
     </row>
     <row r="72" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D72">
         <v>10.7888</v>
@@ -9790,7 +12032,7 @@
     </row>
     <row r="73" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D73">
         <v>2.6092</v>
@@ -9801,7 +12043,7 @@
     </row>
     <row r="74" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D74">
         <v>5.1657999999999999</v>
@@ -9812,7 +12054,7 @@
     </row>
     <row r="80" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D80" t="s">
         <v>8</v>
@@ -9823,7 +12065,7 @@
     </row>
     <row r="81" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D81">
         <v>29.429600000000001</v>
@@ -9834,7 +12076,7 @@
     </row>
     <row r="82" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D82">
         <v>30.133400000000002</v>
@@ -9845,7 +12087,7 @@
     </row>
     <row r="83" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D83">
         <v>3.8187000000000002</v>
@@ -9856,7 +12098,7 @@
     </row>
     <row r="84" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D84">
         <v>20.230499999999999</v>
@@ -9867,7 +12109,7 @@
     </row>
     <row r="85" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C85" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D85">
         <v>13.058199999999999</v>
@@ -9878,7 +12120,7 @@
     </row>
     <row r="86" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C86" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D86">
         <v>3.3292000000000002</v>
@@ -9889,7 +12131,7 @@
     </row>
     <row r="97" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C97" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D97" t="s">
         <v>8</v>
@@ -9900,7 +12142,7 @@
     </row>
     <row r="98" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C98" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D98">
         <v>1.1124000000000001</v>
@@ -9911,7 +12153,7 @@
     </row>
     <row r="99" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C99" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D99">
         <v>3.0865</v>
@@ -9922,7 +12164,7 @@
     </row>
     <row r="100" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C100" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D100">
         <v>11.071999999999999</v>
@@ -9933,7 +12175,7 @@
     </row>
     <row r="101" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C101" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D101">
         <v>0.99509999999999998</v>
@@ -9944,7 +12186,7 @@
     </row>
     <row r="102" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C102" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D102">
         <v>83.733800000000002</v>
@@ -9955,7 +12197,7 @@
     </row>
     <row r="115" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C115" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D115" t="s">
         <v>8</v>
@@ -9966,7 +12208,7 @@
     </row>
     <row r="116" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C116" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D116">
         <v>38.802500000000002</v>
@@ -9977,7 +12219,7 @@
     </row>
     <row r="117" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C117" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D117">
         <v>61.197400000000002</v>
@@ -9988,7 +12230,7 @@
     </row>
     <row r="131" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C131" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D131" t="s">
         <v>8</v>
@@ -9999,7 +12241,7 @@
     </row>
     <row r="132" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C132" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D132">
         <v>4.0000000000000001E-3</v>
@@ -10010,7 +12252,7 @@
     </row>
     <row r="133" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C133" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D133">
         <v>5.6599999999999998E-2</v>
@@ -10021,7 +12263,7 @@
     </row>
     <row r="134" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C134" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D134">
         <v>1.7677</v>
@@ -10032,7 +12274,7 @@
     </row>
     <row r="135" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C135" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D135">
         <v>4.8500000000000001E-2</v>
@@ -10043,7 +12285,7 @@
     </row>
     <row r="136" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C136" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D136">
         <v>0.33169999999999999</v>
@@ -10054,7 +12296,7 @@
     </row>
     <row r="137" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C137" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D137">
         <v>0.22239999999999999</v>
@@ -10065,7 +12307,7 @@
     </row>
     <row r="138" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C138" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D138">
         <v>0.23050000000000001</v>
@@ -10076,7 +12318,7 @@
     </row>
     <row r="139" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C139" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D139">
         <v>0.28310000000000002</v>
@@ -10087,7 +12329,7 @@
     </row>
     <row r="140" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C140" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D140">
         <v>0.27500000000000002</v>
@@ -10098,7 +12340,7 @@
     </row>
     <row r="141" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C141" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D141">
         <v>9.7000000000000003E-2</v>
@@ -10109,7 +12351,7 @@
     </row>
     <row r="142" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C142" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D142">
         <v>0.39229999999999998</v>
@@ -10120,7 +12362,7 @@
     </row>
     <row r="143" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C143" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D143">
         <v>0.2427</v>
@@ -10131,7 +12373,7 @@
     </row>
     <row r="144" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C144" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D144">
         <v>6.8699999999999997E-2</v>
@@ -10142,7 +12384,7 @@
     </row>
     <row r="145" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C145" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D145">
         <v>0.37619999999999998</v>
@@ -10153,7 +12395,7 @@
     </row>
     <row r="146" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C146" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D146">
         <v>8.4900000000000003E-2</v>
@@ -10164,7 +12406,7 @@
     </row>
     <row r="147" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C147" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D147">
         <v>0.2467</v>
@@ -10175,7 +12417,7 @@
     </row>
     <row r="148" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C148" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D148">
         <v>0.1618</v>
@@ -10186,7 +12428,7 @@
     </row>
     <row r="149" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C149" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D149">
         <v>4.8500000000000001E-2</v>
@@ -10197,7 +12439,7 @@
     </row>
     <row r="150" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C150" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D150">
         <v>5.6599999999999998E-2</v>
@@ -10208,7 +12450,7 @@
     </row>
     <row r="151" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C151" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D151">
         <v>4.0399999999999998E-2</v>
@@ -10219,7 +12461,7 @@
     </row>
     <row r="152" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C152" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D152">
         <v>0.2427</v>
@@ -10230,7 +12472,7 @@
     </row>
     <row r="153" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C153" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D153">
         <v>0.1011</v>
@@ -10241,7 +12483,7 @@
     </row>
     <row r="154" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C154" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D154">
         <v>7.6799999999999993E-2</v>
@@ -10252,7 +12494,7 @@
     </row>
     <row r="155" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C155" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D155">
         <v>0.19409999999999999</v>
@@ -10263,7 +12505,7 @@
     </row>
     <row r="156" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C156" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D156">
         <v>0.28720000000000001</v>
@@ -10274,7 +12516,7 @@
     </row>
     <row r="157" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C157" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D157">
         <v>0.1537</v>
@@ -10285,7 +12527,7 @@
     </row>
     <row r="158" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C158" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D158">
         <v>6.4699999999999994E-2</v>
@@ -10296,7 +12538,7 @@
     </row>
     <row r="159" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C159" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D159">
         <v>2.4676</v>
@@ -10307,7 +12549,7 @@
     </row>
     <row r="160" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C160" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D160">
         <v>0.12939999999999999</v>
@@ -10318,7 +12560,7 @@
     </row>
     <row r="161" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C161" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D161">
         <v>0.1173</v>
@@ -10329,7 +12571,7 @@
     </row>
     <row r="162" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C162" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D162">
         <v>0.55420000000000003</v>
@@ -10340,7 +12582,7 @@
     </row>
     <row r="163" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C163" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D163">
         <v>0.19409999999999999</v>
@@ -10351,7 +12593,7 @@
     </row>
     <row r="164" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C164" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D164">
         <v>0.13339999999999999</v>
@@ -10362,7 +12604,7 @@
     </row>
     <row r="165" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C165" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D165">
         <v>0.41260000000000002</v>
@@ -10373,7 +12615,7 @@
     </row>
     <row r="166" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C166" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D166">
         <v>3.6400000000000002E-2</v>
@@ -10384,7 +12626,7 @@
     </row>
     <row r="167" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C167" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D167">
         <v>0.25879999999999997</v>
@@ -10395,7 +12637,7 @@
     </row>
     <row r="168" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C168" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D168">
         <v>0.12540000000000001</v>
@@ -10406,7 +12648,7 @@
     </row>
     <row r="169" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C169" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D169">
         <v>6.0600000000000001E-2</v>
@@ -10417,7 +12659,7 @@
     </row>
     <row r="170" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C170" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D170">
         <v>6.8699999999999997E-2</v>
@@ -10428,7 +12670,7 @@
     </row>
     <row r="171" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C171" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D171">
         <v>0.25080000000000002</v>
@@ -10439,7 +12681,7 @@
     </row>
     <row r="172" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C172" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D172">
         <v>4.0399999999999998E-2</v>
@@ -10448,8 +12690,460 @@
         <v>7.6499999999999999E-2</v>
       </c>
     </row>
+    <row r="176" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C176" t="s">
+        <v>53</v>
+      </c>
+      <c r="D176" t="s">
+        <v>8</v>
+      </c>
+      <c r="E176" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="177" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C177" t="s">
+        <v>68</v>
+      </c>
+      <c r="D177">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="E177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C178" t="s">
+        <v>87</v>
+      </c>
+      <c r="D178">
+        <v>3.6400000000000002E-2</v>
+      </c>
+      <c r="E178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C179" t="s">
+        <v>79</v>
+      </c>
+      <c r="D179">
+        <v>2.0199999999999999E-2</v>
+      </c>
+      <c r="E179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C180" t="s">
+        <v>91</v>
+      </c>
+      <c r="D180">
+        <v>3.2300000000000002E-2</v>
+      </c>
+      <c r="E180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C181" t="s">
+        <v>11</v>
+      </c>
+      <c r="D181">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="E181">
+        <v>0.94369999999999998</v>
+      </c>
+    </row>
+    <row r="182" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C182" t="s">
+        <v>56</v>
+      </c>
+      <c r="D182">
+        <v>2.8299999999999999E-2</v>
+      </c>
+      <c r="E182">
+        <v>2.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="183" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C183" t="s">
+        <v>57</v>
+      </c>
+      <c r="D183">
+        <v>0.14960000000000001</v>
+      </c>
+      <c r="E183">
+        <v>0.30599999999999999</v>
+      </c>
+    </row>
+    <row r="184" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C184" t="s">
+        <v>58</v>
+      </c>
+      <c r="D184">
+        <v>0.12540000000000001</v>
+      </c>
+      <c r="E184">
+        <v>0.20399999999999999</v>
+      </c>
+    </row>
+    <row r="185" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C185" t="s">
+        <v>59</v>
+      </c>
+      <c r="D185">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="E185">
+        <v>2.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="186" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C186" t="s">
+        <v>60</v>
+      </c>
+      <c r="D186">
+        <v>0.13750000000000001</v>
+      </c>
+      <c r="E186">
+        <v>0.1147</v>
+      </c>
+    </row>
+    <row r="187" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C187" t="s">
+        <v>61</v>
+      </c>
+      <c r="D187">
+        <v>0.12130000000000001</v>
+      </c>
+      <c r="E187">
+        <v>3.8199999999999998E-2</v>
+      </c>
+    </row>
+    <row r="188" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C188" t="s">
+        <v>62</v>
+      </c>
+      <c r="D188">
+        <v>6.0600000000000001E-2</v>
+      </c>
+      <c r="E188">
+        <v>2.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="189" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C189" t="s">
+        <v>63</v>
+      </c>
+      <c r="D189">
+        <v>0.19009999999999999</v>
+      </c>
+      <c r="E189">
+        <v>2.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="190" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C190" t="s">
+        <v>64</v>
+      </c>
+      <c r="D190">
+        <v>8.09E-2</v>
+      </c>
+      <c r="E190">
+        <v>0.21679999999999999</v>
+      </c>
+    </row>
+    <row r="191" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C191" t="s">
+        <v>65</v>
+      </c>
+      <c r="D191">
+        <v>2.0199999999999999E-2</v>
+      </c>
+      <c r="E191">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="192" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C192" t="s">
+        <v>66</v>
+      </c>
+      <c r="D192">
+        <v>0.22239999999999999</v>
+      </c>
+      <c r="E192">
+        <v>0.17849999999999999</v>
+      </c>
+    </row>
+    <row r="193" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C193" t="s">
+        <v>67</v>
+      </c>
+      <c r="D193">
+        <v>4.0399999999999998E-2</v>
+      </c>
+      <c r="E193">
+        <v>0.1275</v>
+      </c>
+    </row>
+    <row r="194" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C194" t="s">
+        <v>69</v>
+      </c>
+      <c r="D194">
+        <v>0.1051</v>
+      </c>
+      <c r="E194">
+        <v>6.3700000000000007E-2</v>
+      </c>
+    </row>
+    <row r="195" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C195" t="s">
+        <v>70</v>
+      </c>
+      <c r="D195">
+        <v>2.4199999999999999E-2</v>
+      </c>
+      <c r="E195">
+        <v>1.2699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="196" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C196" t="s">
+        <v>71</v>
+      </c>
+      <c r="D196">
+        <v>3.2300000000000002E-2</v>
+      </c>
+      <c r="E196">
+        <v>2.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="197" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C197" t="s">
+        <v>72</v>
+      </c>
+      <c r="D197">
+        <v>1.21E-2</v>
+      </c>
+      <c r="E197">
+        <v>3.8199999999999998E-2</v>
+      </c>
+    </row>
+    <row r="198" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C198" t="s">
+        <v>73</v>
+      </c>
+      <c r="D198">
+        <v>0.1173</v>
+      </c>
+      <c r="E198">
+        <v>0.28050000000000003</v>
+      </c>
+    </row>
+    <row r="199" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C199" t="s">
+        <v>74</v>
+      </c>
+      <c r="D199">
+        <v>4.8500000000000001E-2</v>
+      </c>
+      <c r="E199">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="200" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C200" t="s">
+        <v>75</v>
+      </c>
+      <c r="D200">
+        <v>2.8299999999999999E-2</v>
+      </c>
+      <c r="E200">
+        <v>7.6499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="201" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C201" t="s">
+        <v>76</v>
+      </c>
+      <c r="D201">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="E201">
+        <v>0.1147</v>
+      </c>
+    </row>
+    <row r="202" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C202" t="s">
+        <v>77</v>
+      </c>
+      <c r="D202">
+        <v>8.09E-2</v>
+      </c>
+      <c r="E202">
+        <v>6.3700000000000007E-2</v>
+      </c>
+    </row>
+    <row r="203" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C203" t="s">
+        <v>78</v>
+      </c>
+      <c r="D203">
+        <v>8.8900000000000007E-2</v>
+      </c>
+      <c r="E203">
+        <v>0.10199999999999999</v>
+      </c>
+    </row>
+    <row r="204" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C204" t="s">
+        <v>80</v>
+      </c>
+      <c r="D204">
+        <v>1.1893</v>
+      </c>
+      <c r="E204">
+        <v>0.17849999999999999</v>
+      </c>
+    </row>
+    <row r="205" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C205" t="s">
+        <v>81</v>
+      </c>
+      <c r="D205">
+        <v>5.6599999999999998E-2</v>
+      </c>
+      <c r="E205">
+        <v>1.2699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="206" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C206" t="s">
+        <v>55</v>
+      </c>
+      <c r="D206">
+        <v>3.2300000000000002E-2</v>
+      </c>
+      <c r="E206">
+        <v>1.2699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="207" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C207" t="s">
+        <v>82</v>
+      </c>
+      <c r="D207">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="E207">
+        <v>2.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="208" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C208" t="s">
+        <v>83</v>
+      </c>
+      <c r="D208">
+        <v>0.29530000000000001</v>
+      </c>
+      <c r="E208">
+        <v>0.30599999999999999</v>
+      </c>
+    </row>
+    <row r="209" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C209" t="s">
+        <v>84</v>
+      </c>
+      <c r="D209">
+        <v>8.8900000000000007E-2</v>
+      </c>
+      <c r="E209">
+        <v>6.3700000000000007E-2</v>
+      </c>
+    </row>
+    <row r="210" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C210" t="s">
+        <v>85</v>
+      </c>
+      <c r="D210">
+        <v>8.8900000000000007E-2</v>
+      </c>
+      <c r="E210">
+        <v>0.10199999999999999</v>
+      </c>
+    </row>
+    <row r="211" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C211" t="s">
+        <v>86</v>
+      </c>
+      <c r="D211">
+        <v>0.25080000000000002</v>
+      </c>
+      <c r="E211">
+        <v>0.10199999999999999</v>
+      </c>
+    </row>
+    <row r="212" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C212" t="s">
+        <v>88</v>
+      </c>
+      <c r="D212">
+        <v>0.12540000000000001</v>
+      </c>
+      <c r="E212">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="213" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C213" t="s">
+        <v>89</v>
+      </c>
+      <c r="D213">
+        <v>3.2300000000000002E-2</v>
+      </c>
+      <c r="E213">
+        <v>7.6499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="214" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C214" t="s">
+        <v>90</v>
+      </c>
+      <c r="D214">
+        <v>4.0399999999999998E-2</v>
+      </c>
+      <c r="E214">
+        <v>2.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="215" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C215" t="s">
+        <v>92</v>
+      </c>
+      <c r="D215">
+        <v>6.8699999999999997E-2</v>
+      </c>
+      <c r="E215">
+        <v>2.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="216" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C216" t="s">
+        <v>93</v>
+      </c>
+      <c r="D216">
+        <v>2.0199999999999999E-2</v>
+      </c>
+      <c r="E216">
+        <v>2.5499999999999998E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>